<commit_message>
feat: add `branch_name` to input search excel
</commit_message>
<xml_diff>
--- a/input_amazon_search.xlsx
+++ b/input_amazon_search.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Software dev\Spyware\DataScraper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srivallabhm/Development/Dev-Projects/Spyware-DataScraper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52DFD5D0-F3E9-4689-8BFE-29A74F467A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C6C308-2DD1-874E-99F2-5F7F68A5A246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>search_keyword</t>
   </si>
@@ -40,6 +40,15 @@
   </si>
   <si>
     <t>Vitamin Deficiency</t>
+  </si>
+  <si>
+    <t>Optimum Nutrition</t>
+  </si>
+  <si>
+    <t>Nature made</t>
+  </si>
+  <si>
+    <t>brand_name</t>
   </si>
 </sst>
 </file>
@@ -357,39 +366,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>